<commit_message>
Excel sheet updated for First Integration
</commit_message>
<xml_diff>
--- a/database/Extraction_data.xlsx
+++ b/database/Extraction_data.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:O730"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -38497,55 +38497,122 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="10.36328125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.26953125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="121.08984375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.90625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.90625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="16.7265625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="8.81640625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="17.54296875" bestFit="1" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>GIE0189</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>AIR HOIST - 1 TONNE - 10MTR HOL C/W 10MTR PENDANT</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>1.00 Tonnes</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+    <row r="1" ht="17" customHeight="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Id Number</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>RFID</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Item Category </t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Item Description </t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>SWL</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>Manufacturer</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>Certificate No</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Detailed Location </t>
+        </is>
+      </c>
+      <c r="K1" s="6" t="inlineStr">
+        <is>
+          <t>Previous Inspection</t>
+        </is>
+      </c>
+      <c r="L1" s="6" t="inlineStr">
+        <is>
+          <t>Next Inspection Due Date</t>
+        </is>
+      </c>
+      <c r="M1" s="6" t="inlineStr">
+        <is>
+          <t>Fit For Purpose Y/N</t>
+        </is>
+      </c>
+      <c r="N1" s="6" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="O1" s="6" t="inlineStr">
+        <is>
+          <t>Provider Identification</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GIT08555</t>
+          <t>GIE0189</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AIR HOIST - 2 TONNE - 15MTR HOL C/W 10MTR PENDANT</t>
-        </is>
-      </c>
+          <t>AIR HOIST - 1 TONNE - 10MTR HOL C/W 10MTR PENDANT</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.00 Tonnes</t>
+          <t>1.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -38557,19 +38624,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GIT26471</t>
+          <t>GIT08555</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ANGLE CLAMP - 1 TONNE AC2 - 38-101MM</t>
-        </is>
-      </c>
+          <t>AIR HOIST - 2 TONNE - 15MTR HOL C/W 10MTR PENDANT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.00 Tonnes</t>
-        </is>
-      </c>
+          <t>2.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38579,7 +38648,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GIT26472</t>
+          <t>GIT26471</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -38587,11 +38656,17 @@
           <t>ANGLE CLAMP - 1 TONNE AC2 - 38-101MM</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>AC2</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38601,19 +38676,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GIT18457</t>
+          <t>GIT26472</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
+          <t>ANGLE CLAMP - 1 TONNE AC2 - 38-101MM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AC2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>3.00 Tonnes</t>
-        </is>
-      </c>
+          <t>1.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38623,7 +38704,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GIT20245</t>
+          <t>GIT18457</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -38631,11 +38712,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38645,7 +38732,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GIT20723</t>
+          <t>GIT20245</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -38653,16 +38740,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38672,7 +38760,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GIT20263</t>
+          <t>GIT20723</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -38680,11 +38768,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38699,7 +38793,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GIT21153</t>
+          <t>GIT20263</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -38707,11 +38801,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38726,7 +38826,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GIT20164</t>
+          <t>GIT21153</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -38734,11 +38834,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38753,7 +38859,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GIT20140</t>
+          <t>GIT20164</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -38761,11 +38867,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38780,7 +38892,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GIT18453</t>
+          <t>GIT20140</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -38788,11 +38900,17 @@
           <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38807,17 +38925,28 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GIT03864</t>
+          <t>GIT18453</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>BEAM TROLLEY 6 TONNE - B2 - 105 - 305MM</t>
+          <t>BEAM CLAMP - 3 TONNE BCU-0300 125-204MM</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BCU-0300</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6.00 Tonnes</t>
+          <t>3.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -38829,24 +38958,25 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GIT06483</t>
+          <t>GIT03864</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 1 TONNE X 3MTR</t>
+          <t>BEAM TROLLEY 6 TONNE - B2 - 105 - 305MM</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>B2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1.00 Tonnes</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
+          <t>6.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38856,7 +38986,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GIT20474</t>
+          <t>GIT06483</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -38864,11 +38994,13 @@
           <t>CHAIN BLOCK 1 TONNE X 3MTR</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38883,7 +39015,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GIT21573</t>
+          <t>GIT20474</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -38891,11 +39023,13 @@
           <t>CHAIN BLOCK 1 TONNE X 3MTR</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38910,7 +39044,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GIT22412</t>
+          <t>GIT21573</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -38918,11 +39052,13 @@
           <t>CHAIN BLOCK 1 TONNE X 3MTR</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -38937,17 +39073,24 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GIT20005</t>
+          <t>GIT22412</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 1 TONNE X 6MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 1 TONNE X 3MTR</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -38959,7 +39102,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GIT10519</t>
+          <t>GIT20005</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -38967,11 +39110,13 @@
           <t>CHAIN BLOCK 1 TONNE X 6MTR</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -38981,7 +39126,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GIT08203</t>
+          <t>GIT10519</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -38989,11 +39134,13 @@
           <t>CHAIN BLOCK 1 TONNE X 6MTR</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
           <t>1.00 Tonnes</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39003,24 +39150,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GIT18866</t>
+          <t>GIT08203</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 250 KGS X 3MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 1 TONNE X 6MTR</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>250.00 Kilos</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
+          <t>1.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39030,7 +39174,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GIT18882</t>
+          <t>GIT18866</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -39038,11 +39182,13 @@
           <t>CHAIN BLOCK 250 KGS X 3MTR</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
           <t>250.00 Kilos</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -39057,17 +39203,24 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GIT17038</t>
+          <t>GIT18882</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 250 KGS X 6MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 250 KGS X 3MTR</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
           <t>250.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -39079,7 +39232,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GIT18901</t>
+          <t>GIT17038</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -39087,11 +39240,13 @@
           <t>CHAIN BLOCK 250 KGS X 6MTR</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
           <t>250.00 Kilos</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39101,19 +39256,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GIT04245</t>
+          <t>GIT18901</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 5 TONNE X 6MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 250 KGS X 6MTR</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>5.00 Tonnes</t>
-        </is>
-      </c>
+          <t>250.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39123,7 +39280,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GIT04837</t>
+          <t>GIT04245</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -39131,11 +39288,13 @@
           <t>CHAIN BLOCK 5 TONNE X 6MTR</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>5.00 Tonnes</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39145,24 +39304,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GIT18838</t>
+          <t>GIT04837</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 500 KGS X 3MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 5 TONNE X 6MTR</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>500.00 Kilos</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
+          <t>5.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39172,7 +39328,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GIT20737</t>
+          <t>GIT18838</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -39180,11 +39336,13 @@
           <t>CHAIN BLOCK 500 KGS X 3MTR</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>500.00 Kilos</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
           <t>ABZ/011196/39693</t>
@@ -39199,17 +39357,24 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GIT22633</t>
+          <t>GIT20737</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>CHAIN BLOCK 500 KGS X 6MTR</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 500 KGS X 3MTR</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>500.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -39221,7 +39386,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GIT12801</t>
+          <t>GIT22633</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -39229,11 +39394,13 @@
           <t>CHAIN BLOCK 500 KGS X 6MTR</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>500.00 Kilos</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39243,19 +39410,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GIT26457</t>
+          <t>GIT12801</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>INERTIA REEL -RGA3.3 GALV FALL ARREST BLOCK</t>
-        </is>
-      </c>
+          <t>CHAIN BLOCK 500 KGS X 6MTR</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>136.00 Kilos</t>
-        </is>
-      </c>
+          <t>500.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39265,19 +39434,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GIT22778</t>
+          <t>GIT26457</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PULL LIFT 1.6 TONNE X 3MTR</t>
-        </is>
-      </c>
+          <t>INERTIA REEL -RGA3.3 GALV FALL ARREST BLOCK</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1.60 Tonnes</t>
-        </is>
-      </c>
+          <t>136.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39287,7 +39458,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GIT06431</t>
+          <t>GIT22778</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -39295,16 +39466,13 @@
           <t>PULL LIFT 1.6 TONNE X 3MTR</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
           <t>1.60 Tonnes</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>ABZ/011196/39693</t>
-        </is>
-      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39314,17 +39482,24 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GIT22544</t>
+          <t>GIT06431</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PULL LIFT 800 KGS X 1.5MTR</t>
-        </is>
-      </c>
+          <t>PULL LIFT 1.6 TONNE X 3MTR</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>750.00 Kilos</t>
+          <t>1.60 Tonnes</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>ABZ/011196/39693</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -39336,7 +39511,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GIT19762</t>
+          <t>GIT22544</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -39344,11 +39519,13 @@
           <t>PULL LIFT 800 KGS X 1.5MTR</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
           <t>750.00 Kilos</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39358,19 +39535,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GIT26459</t>
+          <t>GIT19762</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
-        </is>
-      </c>
+          <t>PULL LIFT 800 KGS X 1.5MTR</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>136.00 Kilos</t>
-        </is>
-      </c>
+          <t>750.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39380,19 +39559,25 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GIT22352</t>
+          <t>GIT26459</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">SNATCH BLOCK 4 TONNE 4.5" </t>
+          <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>RGA4</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>4.00 Tonnes</t>
-        </is>
-      </c>
+          <t>136.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39402,19 +39587,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GIT06408</t>
+          <t>GIT22352</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>TIRFOR MACHINE 3.2 TONNE C/W HANDLE</t>
-        </is>
-      </c>
+          <t xml:space="preserve">SNATCH BLOCK 4 TONNE 4.5" </t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>3.20 Tonnes</t>
-        </is>
-      </c>
+          <t>4.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39424,19 +39611,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GIT04707</t>
+          <t>GIT06408</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>TIRFOR ROPE 3.2 TONNE X 20MTR</t>
-        </is>
-      </c>
+          <t>TIRFOR MACHINE 3.2 TONNE C/W HANDLE</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
           <t>3.20 Tonnes</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39446,24 +39635,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GIA0615</t>
+          <t>GIT04707</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">6" SNATCH BLOCK 8 TONNE </t>
-        </is>
-      </c>
+          <t>TIRFOR ROPE 3.2 TONNE X 20MTR</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>8.00 Tonnes</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>ABZ/011208/39714</t>
-        </is>
-      </c>
+          <t>3.20 Tonnes</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39473,7 +39659,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GIA0664</t>
+          <t>GIA0615</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -39481,11 +39667,13 @@
           <t xml:space="preserve">6" SNATCH BLOCK 8 TONNE </t>
         </is>
       </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>8.00 Tonnes</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
           <t>ABZ/011208/39714</t>
@@ -39500,17 +39688,24 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GIT09372</t>
+          <t>GIA0664</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>AIR HOIST - 3 TONNE - 15MTR HOL - 15MTR PENDANT</t>
-        </is>
-      </c>
+          <t xml:space="preserve">6" SNATCH BLOCK 8 TONNE </t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>3.00 Tonnes</t>
+          <t>8.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>ABZ/011208/39714</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -39522,7 +39717,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GIT06791</t>
+          <t>GIT09372</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -39530,11 +39725,13 @@
           <t>AIR HOIST - 3 TONNE - 15MTR HOL - 15MTR PENDANT</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39544,106 +39741,109 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>GIT06791</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>AIR HOIST - 3 TONNE - 15MTR HOL - 15MTR PENDANT</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>3.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>GIT11821</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Name &amp; qualifications of person making the report
 Date of thorough examination: 18/08/2023  Name of the person authenticating this report</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="G45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
         <is>
           <t>18/08/2023</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>17/03/2024</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="46">
+      <c r="A46" t="inlineStr">
         <is>
           <t>GIT03785</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Name &amp; qualifications of person making the report
 Date of thorough examination: 18/08/2023  Name of the person authenticating this report</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="G46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
         <is>
           <t>18/08/2023</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>17/03/2024</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>GIT20196</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Name &amp; qualifications of person making the report
 Date of thorough examination: 18/08/2023  Name of the person authenticating this report</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
         <is>
           <t>3.00 Tonnes</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="G47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
         <is>
           <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>GIT26458</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>136.00 Kilos</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>ABZ/011208/39714</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -39655,7 +39855,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GIT26460</t>
+          <t>GIT26458</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -39663,11 +39863,17 @@
           <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>RGA4</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>136.00 Kilos</t>
         </is>
       </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
           <t>ABZ/011208/39714</t>
@@ -39682,7 +39888,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>GIT26461</t>
+          <t>GIT26460</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -39690,11 +39896,17 @@
           <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>RGA4</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>136.00 Kilos</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
           <t>ABZ/011208/39714</t>
@@ -39709,7 +39921,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>GIT26462</t>
+          <t>GIT26461</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -39717,11 +39929,17 @@
           <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>RGA4</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>136.00 Kilos</t>
         </is>
       </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
           <t>ABZ/011208/39714</t>
@@ -39736,17 +39954,28 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>GIT12528</t>
+          <t>GIT26462</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">SNATCH BLOCK 4 TONNE 4.5" </t>
+          <t>RETRIEVEABLE INERTIA REEL RGA4 - 15MTR</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>RGA4</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>4.00 Tonnes</t>
+          <t>136.00 Kilos</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>ABZ/011208/39714</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -39758,7 +39987,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>GIA0714</t>
+          <t>GIT12528</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -39766,11 +39995,13 @@
           <t xml:space="preserve">SNATCH BLOCK 4 TONNE 4.5" </t>
         </is>
       </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
           <t>4.00 Tonnes</t>
         </is>
       </c>
+      <c r="G52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
           <t>17/03/2024</t>
@@ -39780,296 +40011,2656 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>GIA0714</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SNATCH BLOCK 4 TONNE 4.5" </t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>4.00 Tonnes</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>GIT09442</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>Name &amp; qualifications of person making the report
 Date of thorough examination: 18/08/2023  Name of the person authenticating this report</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
         <is>
           <t>5.00 Tonnes</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr">
+      <c r="G54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
         <is>
           <t>18/08/2023</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
+      <c r="L54" t="inlineStr">
         <is>
           <t>17/03/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>SYE1-10</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>1 TONNE</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>SYE44-59</t>
+          <t>SYE1</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>ABZ/539613/0008</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>SYE88-89</t>
+          <t>SYE2</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>5TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>ABZ/539613/0014</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>R1/185308/01-06</t>
+          <t>SYE3</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
           <t>1 TONNE</t>
         </is>
       </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>ABZ/539613/0015</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>R3/185296/01-10</t>
+          <t>SYE4</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>3TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>ABZ/539613/0027</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SYE172-177</t>
+          <t>SYE5</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>6 X A344 17MM MASTER LINK</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>4.1TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>ABZ/539613/0030</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SYE90-99</t>
+          <t>SYE6</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>1TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>ABZ/539613/0031</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>SYE148-165</t>
+          <t>SYE7</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>3.25TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>ABZ/539613/0037</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>18/08/2023</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>17/03/2024</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TAA1-2</t>
+          <t>SYE8</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
-        </is>
-      </c>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>8 TONNE</t>
-        </is>
-      </c>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>ABZ/539976/0001</t>
+          <t>ABZ/539613/0002</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>TAA3-4</t>
+          <t>SYE9</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0002</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SYE10</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>10 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0002</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SYE44</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>SYE45</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SYE46</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SYE47</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>SYE48</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SYE49</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>SYE50</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>SYE51</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SYE52</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>SYE53</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>SYE54</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SYE55</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SYE56</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>SYE57</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>SYE58</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SYE59</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>16X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>2TONNE</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0008</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>SYE88</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>5TONNE</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0014</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>SYE89</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>5TONNE</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0014</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>R1/1853081</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>R1/1853082</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>R1/1853083</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>R1/1853084</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>R1/1853085</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>R1/1853086</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>6 X 1 TONNE X 0.5MTR EWL ROUND SLING (1MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>1 TONNE</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0015</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>R3/1852961</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>R3/1852962</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>R3/1852963</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>R3/1852964</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>R3/1852965</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>R3/1852966</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>R3/1852967</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>R3/1852968</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>R3/1852969</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>R3/18529610</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>10X3TONNE X5MTR EWL ROUND SLING (10MTR CIRC)</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>3TONNE</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0027</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>SYE172</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>SYE173</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>SYE174</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>SYE175</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>SYE176</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SYE177</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>6 X A344 17MM MASTER LINK</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>A344</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>4.1TONNE</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0030</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>SYE90</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>SYE91</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>SYE92</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SYE93</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>SYE94</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>SYE95</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>SYE96</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>SYE97</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>SYE98</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>SYE99</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>10 X 1 TONNE SCREW PIN BOW SHACKLE G-209</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>G-209</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>1TONNE</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0031</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>SYE148</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>SYE149</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>SYE150</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>SYE151</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SYE152</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SYE153</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SYE154</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SYE155</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SYE156</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>SYE157</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>SYE158</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>SYE159</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>SYE160</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>SYE161</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>SYE162</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>SYE163</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>SYE164</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>SYE165</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>18 X 3.25 TONNE SAFETY PIN BOW SHACKLE G-2130</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>G-2130</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>3.25TONNE</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>ABZ/539613/0037</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>17/03/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>TAA1</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
           <t>2 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr">
         <is>
           <t>8 TONNE</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>ABZ/539976/0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>TAA2</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>8 TONNE</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>ABZ/539976/0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>TAA3</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>8 TONNE</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>ABZ/539976/0002</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>TAA4</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2 X SINGLE LEG WIRE ROPE SLING TO BS EN 13414-1</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>8 TONNE</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr">
         <is>
           <t>ABZ/539976/0002</t>
         </is>

</xml_diff>

<commit_message>
Code changes made for SWL, Model and Manufacture columns for First Integrated
</commit_message>
<xml_diff>
--- a/database/Extraction_data.xlsx
+++ b/database/Extraction_data.xlsx
@@ -38685,11 +38685,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
@@ -38729,11 +38724,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
@@ -38773,11 +38763,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
@@ -38817,11 +38802,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
@@ -38865,12 +38845,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -38913,12 +38892,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -38961,12 +38939,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -39009,12 +38986,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -39057,12 +39033,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -39105,12 +39080,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -39153,12 +39127,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -39197,11 +39170,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
@@ -39241,11 +39209,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
@@ -39285,11 +39248,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
@@ -39329,11 +39287,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
@@ -39373,11 +39326,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
@@ -39417,11 +39365,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
@@ -39461,11 +39404,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
@@ -39505,11 +39443,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
@@ -39549,11 +39482,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
@@ -39593,11 +39521,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
@@ -39637,11 +39560,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
@@ -39681,11 +39599,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
@@ -39725,11 +39638,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
@@ -39769,11 +39677,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
@@ -39813,11 +39716,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
@@ -39857,11 +39755,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
@@ -39901,11 +39794,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
@@ -39945,11 +39833,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
@@ -39989,11 +39872,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
@@ -40033,11 +39911,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
@@ -40077,11 +39950,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
@@ -40121,11 +39989,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
@@ -40165,11 +40028,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
@@ -40209,11 +40067,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
@@ -40253,11 +40106,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
@@ -40297,11 +40145,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
@@ -40345,12 +40188,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40393,12 +40235,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40441,12 +40282,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J41" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40489,12 +40329,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J42" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40537,12 +40376,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J43" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40585,12 +40423,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J44" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40633,12 +40470,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40677,11 +40513,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr">
         <is>
@@ -40721,11 +40552,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
@@ -40769,12 +40595,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40817,12 +40642,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr">
         <is>
           <t>ABZ/012186/43094</t>
@@ -40861,11 +40685,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
@@ -40905,11 +40724,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr">
         <is>
@@ -40949,11 +40763,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
@@ -40993,11 +40802,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
@@ -41041,12 +40845,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J54" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41089,12 +40892,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J55" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41137,12 +40939,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41185,12 +40986,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41233,12 +41033,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J58" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41281,12 +41080,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41329,12 +41127,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J60" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41377,12 +41174,11 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Tiger</t>
+        </is>
+      </c>
       <c r="J61" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -41421,11 +41217,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
@@ -41465,11 +41256,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr">
         <is>
@@ -41509,11 +41295,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
@@ -41553,11 +41334,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
@@ -41597,11 +41373,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
@@ -41641,11 +41412,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
@@ -41685,11 +41451,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr">
         <is>
@@ -41729,11 +41490,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
@@ -41773,11 +41529,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr">
         <is>
@@ -41817,11 +41568,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
@@ -41861,11 +41607,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
@@ -41905,11 +41646,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr">
         <is>
@@ -41949,11 +41685,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr">
         <is>
@@ -41993,11 +41724,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
@@ -42037,11 +41763,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr">
         <is>
@@ -42081,11 +41802,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr">
         <is>
@@ -42125,11 +41841,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr">
         <is>
@@ -42169,11 +41880,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr">
         <is>
@@ -42213,11 +41919,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr">
         <is>
@@ -42257,11 +41958,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr">
         <is>
@@ -42301,11 +41997,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
@@ -42345,11 +42036,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr">
         <is>
@@ -42389,11 +42075,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr">
         <is>
@@ -42424,7 +42105,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>RHINO</t>
+          <t>BLACK RHINO</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -42437,12 +42118,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Miller</t>
+        </is>
+      </c>
       <c r="J85" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -42481,11 +42161,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr">
         <is>
@@ -42525,11 +42200,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr">
         <is>
@@ -42569,11 +42239,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr">
         <is>
@@ -42613,11 +42278,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr">
         <is>
@@ -42657,11 +42317,6 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr">
         <is>
@@ -42705,12 +42360,11 @@
           <t>Kilos</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Kilos</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr"/>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Ridge Gear</t>
+        </is>
+      </c>
       <c r="J91" t="inlineStr">
         <is>
           <t>ABZ/012185/43140</t>
@@ -42749,11 +42403,6 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr">
         <is>
@@ -42797,14 +42446,9 @@
           <t>Tonnes</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>Superclamp</t>
+          <t xml:space="preserve">Riley </t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -42841,11 +42485,6 @@
         </is>
       </c>
       <c r="G94" t="inlineStr">
-        <is>
-          <t>Tonnes</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
         <is>
           <t>Tonnes</t>
         </is>
@@ -51564,11 +51203,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E330" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E330" t="inlineStr"/>
       <c r="F330" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51607,11 +51242,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E331" t="inlineStr"/>
       <c r="F331" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51650,11 +51281,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E332" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E332" t="inlineStr"/>
       <c r="F332" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51693,11 +51320,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E333" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E333" t="inlineStr"/>
       <c r="F333" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51736,11 +51359,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E334" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E334" t="inlineStr"/>
       <c r="F334" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51779,11 +51398,7 @@
           <t>6 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E335" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E335" t="inlineStr"/>
       <c r="F335" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -51837,7 +51452,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I336" t="inlineStr"/>
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J336" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -51880,7 +51499,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I337" t="inlineStr"/>
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J337" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -51923,7 +51546,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I338" t="inlineStr"/>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J338" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -51966,7 +51593,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I339" t="inlineStr"/>
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J339" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52009,7 +51640,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I340" t="inlineStr"/>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J340" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52052,7 +51687,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I341" t="inlineStr"/>
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J341" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52095,7 +51734,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I342" t="inlineStr"/>
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J342" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52138,7 +51781,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I343" t="inlineStr"/>
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J343" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52181,7 +51828,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I344" t="inlineStr"/>
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J344" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52224,7 +51875,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I345" t="inlineStr"/>
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J345" t="inlineStr">
         <is>
           <t>ABZ/543069/0031</t>
@@ -52267,7 +51922,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I346" t="inlineStr"/>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J346" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52310,7 +51969,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I347" t="inlineStr"/>
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J347" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52353,7 +52016,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I348" t="inlineStr"/>
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J348" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52396,7 +52063,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I349" t="inlineStr"/>
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J349" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52439,7 +52110,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I350" t="inlineStr"/>
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J350" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52482,7 +52157,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I351" t="inlineStr"/>
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J351" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52525,7 +52204,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I352" t="inlineStr"/>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J352" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52568,7 +52251,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I353" t="inlineStr"/>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J353" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52611,7 +52298,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I354" t="inlineStr"/>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J354" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52654,7 +52345,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I355" t="inlineStr"/>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J355" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52697,7 +52392,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I356" t="inlineStr"/>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J356" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52740,7 +52439,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I357" t="inlineStr"/>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J357" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52783,7 +52486,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I358" t="inlineStr"/>
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J358" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52826,7 +52533,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I359" t="inlineStr"/>
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J359" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52869,7 +52580,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I360" t="inlineStr"/>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J360" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52912,7 +52627,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I361" t="inlineStr"/>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J361" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52955,7 +52674,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I362" t="inlineStr"/>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J362" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -52998,7 +52721,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I363" t="inlineStr"/>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J363" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -53041,7 +52768,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I364" t="inlineStr"/>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J364" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -53084,7 +52815,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I365" t="inlineStr"/>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J365" t="inlineStr">
         <is>
           <t>ABZ/543069/0032</t>
@@ -53127,7 +52862,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I366" t="inlineStr"/>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J366" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53170,7 +52909,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I367" t="inlineStr"/>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J367" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53213,7 +52956,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I368" t="inlineStr"/>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J368" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53256,7 +53003,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I369" t="inlineStr"/>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J369" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53299,7 +53050,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I370" t="inlineStr"/>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J370" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53342,7 +53097,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I371" t="inlineStr"/>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J371" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53385,7 +53144,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I372" t="inlineStr"/>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J372" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53428,7 +53191,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I373" t="inlineStr"/>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J373" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53471,7 +53238,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I374" t="inlineStr"/>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J374" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53514,7 +53285,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I375" t="inlineStr"/>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J375" t="inlineStr">
         <is>
           <t>ABZ/543069/0033</t>
@@ -53557,7 +53332,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I376" t="inlineStr"/>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J376" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53600,7 +53379,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I377" t="inlineStr"/>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J377" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53643,7 +53426,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I378" t="inlineStr"/>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J378" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53686,7 +53473,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I379" t="inlineStr"/>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J379" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53729,7 +53520,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I380" t="inlineStr"/>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J380" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53772,7 +53567,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I381" t="inlineStr"/>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J381" t="inlineStr">
         <is>
           <t>ABZ/543069/0034</t>
@@ -53815,7 +53614,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I382" t="inlineStr"/>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J382" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -53858,7 +53661,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I383" t="inlineStr"/>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J383" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -53901,7 +53708,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I384" t="inlineStr"/>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J384" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -53944,7 +53755,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I385" t="inlineStr"/>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J385" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -53987,7 +53802,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I386" t="inlineStr"/>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J386" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -54030,7 +53849,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I387" t="inlineStr"/>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J387" t="inlineStr">
         <is>
           <t>ABZ/543069/0035</t>
@@ -54073,7 +53896,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I388" t="inlineStr"/>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J388" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54116,7 +53943,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I389" t="inlineStr"/>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J389" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54159,7 +53990,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I390" t="inlineStr"/>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J390" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54202,7 +54037,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I391" t="inlineStr"/>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J391" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54245,7 +54084,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I392" t="inlineStr"/>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J392" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54288,7 +54131,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I393" t="inlineStr"/>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J393" t="inlineStr">
         <is>
           <t>ABZ/543069/0036</t>
@@ -54331,7 +54178,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I394" t="inlineStr"/>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J394" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54374,7 +54225,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I395" t="inlineStr"/>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J395" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54417,7 +54272,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I396" t="inlineStr"/>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J396" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54460,7 +54319,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I397" t="inlineStr"/>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J397" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54503,7 +54366,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I398" t="inlineStr"/>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J398" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54546,7 +54413,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I399" t="inlineStr"/>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J399" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54589,7 +54460,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I400" t="inlineStr"/>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J400" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54632,7 +54507,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I401" t="inlineStr"/>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J401" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54675,7 +54554,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I402" t="inlineStr"/>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J402" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54718,7 +54601,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I403" t="inlineStr"/>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J403" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54761,7 +54648,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I404" t="inlineStr"/>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J404" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54804,7 +54695,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I405" t="inlineStr"/>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J405" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54847,7 +54742,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I406" t="inlineStr"/>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J406" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54890,7 +54789,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I407" t="inlineStr"/>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J407" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54933,7 +54836,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I408" t="inlineStr"/>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J408" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -54976,7 +54883,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I409" t="inlineStr"/>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J409" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -55019,7 +54930,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I410" t="inlineStr"/>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J410" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -55062,7 +54977,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I411" t="inlineStr"/>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J411" t="inlineStr">
         <is>
           <t>ABZ/543069/0037</t>
@@ -55105,7 +55024,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I412" t="inlineStr"/>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J412" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -55148,7 +55071,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I413" t="inlineStr"/>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J413" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -55191,7 +55118,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I414" t="inlineStr"/>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J414" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -55234,7 +55165,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I415" t="inlineStr"/>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J415" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -55277,7 +55212,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I416" t="inlineStr"/>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J416" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -55320,7 +55259,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I417" t="inlineStr"/>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J417" t="inlineStr">
         <is>
           <t>ABZ/543069/0038</t>
@@ -60771,7 +60714,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I565" t="inlineStr"/>
+      <c r="I565" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J565" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -60814,7 +60761,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I566" t="inlineStr"/>
+      <c r="I566" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J566" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -60857,7 +60808,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I567" t="inlineStr"/>
+      <c r="I567" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J567" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -60900,7 +60855,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I568" t="inlineStr"/>
+      <c r="I568" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J568" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -60943,7 +60902,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I569" t="inlineStr"/>
+      <c r="I569" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J569" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -60986,7 +60949,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I570" t="inlineStr"/>
+      <c r="I570" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J570" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61029,7 +60996,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I571" t="inlineStr"/>
+      <c r="I571" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J571" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61072,7 +61043,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I572" t="inlineStr"/>
+      <c r="I572" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J572" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61115,7 +61090,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I573" t="inlineStr"/>
+      <c r="I573" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J573" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61158,7 +61137,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I574" t="inlineStr"/>
+      <c r="I574" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J574" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61201,7 +61184,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I575" t="inlineStr"/>
+      <c r="I575" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J575" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61244,7 +61231,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I576" t="inlineStr"/>
+      <c r="I576" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J576" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61287,7 +61278,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I577" t="inlineStr"/>
+      <c r="I577" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J577" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61330,7 +61325,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I578" t="inlineStr"/>
+      <c r="I578" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J578" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61373,7 +61372,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I579" t="inlineStr"/>
+      <c r="I579" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J579" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61416,7 +61419,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I580" t="inlineStr"/>
+      <c r="I580" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J580" t="inlineStr">
         <is>
           <t>ABZ/543074/0024</t>
@@ -61459,7 +61466,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I581" t="inlineStr"/>
+      <c r="I581" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J581" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61502,7 +61513,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I582" t="inlineStr"/>
+      <c r="I582" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J582" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61545,7 +61560,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I583" t="inlineStr"/>
+      <c r="I583" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J583" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61588,7 +61607,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I584" t="inlineStr"/>
+      <c r="I584" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J584" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61631,7 +61654,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I585" t="inlineStr"/>
+      <c r="I585" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J585" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61674,7 +61701,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I586" t="inlineStr"/>
+      <c r="I586" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J586" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61717,7 +61748,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I587" t="inlineStr"/>
+      <c r="I587" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J587" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61760,7 +61795,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I588" t="inlineStr"/>
+      <c r="I588" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J588" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61803,7 +61842,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I589" t="inlineStr"/>
+      <c r="I589" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J589" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61846,7 +61889,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I590" t="inlineStr"/>
+      <c r="I590" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J590" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61889,7 +61936,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I591" t="inlineStr"/>
+      <c r="I591" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J591" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61932,7 +61983,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I592" t="inlineStr"/>
+      <c r="I592" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J592" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -61975,7 +62030,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I593" t="inlineStr"/>
+      <c r="I593" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J593" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62018,7 +62077,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I594" t="inlineStr"/>
+      <c r="I594" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J594" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62061,7 +62124,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I595" t="inlineStr"/>
+      <c r="I595" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J595" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62104,7 +62171,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I596" t="inlineStr"/>
+      <c r="I596" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J596" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62147,7 +62218,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I597" t="inlineStr"/>
+      <c r="I597" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J597" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62190,7 +62265,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I598" t="inlineStr"/>
+      <c r="I598" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J598" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62233,7 +62312,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I599" t="inlineStr"/>
+      <c r="I599" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J599" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62276,7 +62359,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I600" t="inlineStr"/>
+      <c r="I600" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J600" t="inlineStr">
         <is>
           <t>ABZ/543074/0025</t>
@@ -62319,7 +62406,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I601" t="inlineStr"/>
+      <c r="I601" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J601" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62362,7 +62453,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I602" t="inlineStr"/>
+      <c r="I602" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J602" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62405,7 +62500,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I603" t="inlineStr"/>
+      <c r="I603" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J603" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62448,7 +62547,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I604" t="inlineStr"/>
+      <c r="I604" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J604" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62491,7 +62594,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I605" t="inlineStr"/>
+      <c r="I605" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J605" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62534,7 +62641,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I606" t="inlineStr"/>
+      <c r="I606" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J606" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62577,7 +62688,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I607" t="inlineStr"/>
+      <c r="I607" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J607" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62620,7 +62735,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I608" t="inlineStr"/>
+      <c r="I608" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J608" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62663,7 +62782,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I609" t="inlineStr"/>
+      <c r="I609" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J609" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62706,7 +62829,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I610" t="inlineStr"/>
+      <c r="I610" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J610" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62749,7 +62876,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I611" t="inlineStr"/>
+      <c r="I611" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J611" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62792,7 +62923,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I612" t="inlineStr"/>
+      <c r="I612" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J612" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62835,7 +62970,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I613" t="inlineStr"/>
+      <c r="I613" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J613" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62878,7 +63017,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I614" t="inlineStr"/>
+      <c r="I614" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J614" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62921,7 +63064,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I615" t="inlineStr"/>
+      <c r="I615" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J615" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -62964,7 +63111,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I616" t="inlineStr"/>
+      <c r="I616" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J616" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -63007,7 +63158,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I617" t="inlineStr"/>
+      <c r="I617" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J617" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -63050,7 +63205,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I618" t="inlineStr"/>
+      <c r="I618" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J618" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -63093,7 +63252,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I619" t="inlineStr"/>
+      <c r="I619" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J619" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -63136,7 +63299,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I620" t="inlineStr"/>
+      <c r="I620" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J620" t="inlineStr">
         <is>
           <t>ABZ/543074/0026</t>
@@ -63179,7 +63346,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I621" t="inlineStr"/>
+      <c r="I621" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J621" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63222,7 +63393,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I622" t="inlineStr"/>
+      <c r="I622" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J622" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63265,7 +63440,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I623" t="inlineStr"/>
+      <c r="I623" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J623" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63308,7 +63487,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I624" t="inlineStr"/>
+      <c r="I624" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J624" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63351,7 +63534,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I625" t="inlineStr"/>
+      <c r="I625" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J625" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63394,7 +63581,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I626" t="inlineStr"/>
+      <c r="I626" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J626" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63437,7 +63628,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I627" t="inlineStr"/>
+      <c r="I627" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J627" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63480,7 +63675,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I628" t="inlineStr"/>
+      <c r="I628" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J628" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63523,7 +63722,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I629" t="inlineStr"/>
+      <c r="I629" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J629" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63566,7 +63769,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I630" t="inlineStr"/>
+      <c r="I630" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J630" t="inlineStr">
         <is>
           <t>ABZ/543074/0027</t>
@@ -63609,7 +63816,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I631" t="inlineStr"/>
+      <c r="I631" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J631" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63652,7 +63863,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I632" t="inlineStr"/>
+      <c r="I632" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J632" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63695,7 +63910,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I633" t="inlineStr"/>
+      <c r="I633" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J633" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63738,7 +63957,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I634" t="inlineStr"/>
+      <c r="I634" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J634" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63781,7 +64004,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I635" t="inlineStr"/>
+      <c r="I635" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J635" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63824,7 +64051,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I636" t="inlineStr"/>
+      <c r="I636" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J636" t="inlineStr">
         <is>
           <t>ABZ/543074/0028</t>
@@ -63867,7 +64098,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I637" t="inlineStr"/>
+      <c r="I637" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J637" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -63910,7 +64145,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I638" t="inlineStr"/>
+      <c r="I638" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J638" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -63953,7 +64192,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I639" t="inlineStr"/>
+      <c r="I639" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J639" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -63996,7 +64239,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I640" t="inlineStr"/>
+      <c r="I640" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J640" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -64039,7 +64286,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I641" t="inlineStr"/>
+      <c r="I641" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J641" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -64082,7 +64333,11 @@
           <t>TONNE</t>
         </is>
       </c>
-      <c r="I642" t="inlineStr"/>
+      <c r="I642" t="inlineStr">
+        <is>
+          <t>Crosby</t>
+        </is>
+      </c>
       <c r="J642" t="inlineStr">
         <is>
           <t>ABZ/543074/0029</t>
@@ -64110,11 +64365,7 @@
           <t>4 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E643" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E643" t="inlineStr"/>
       <c r="F643" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -64153,11 +64404,7 @@
           <t>4 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E644" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E644" t="inlineStr"/>
       <c r="F644" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -64196,11 +64443,7 @@
           <t>4 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E645" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E645" t="inlineStr"/>
       <c r="F645" t="inlineStr">
         <is>
           <t>4.1</t>
@@ -64239,11 +64482,7 @@
           <t>4 X A344 17MM MASTER LINK</t>
         </is>
       </c>
-      <c r="E646" t="inlineStr">
-        <is>
-          <t>A344</t>
-        </is>
-      </c>
+      <c r="E646" t="inlineStr"/>
       <c r="F646" t="inlineStr">
         <is>
           <t>4.1</t>

</xml_diff>